<commit_message>
processing to get transported sizes!!!!!!
:D
</commit_message>
<xml_diff>
--- a/Hydrophones/Results/noise_corrected/calculations/storm2_results.xlsx
+++ b/Hydrophones/Results/noise_corrected/calculations/storm2_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Hydrophones\Results\noise_corrected\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75698EE-2FBA-4517-AD0A-B15E42B4BE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFDAC65-1328-4790-8199-40F6DE1E8C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{867F3169-A9A3-4AE6-89E2-304587BC45FE}"/>
+    <workbookView xWindow="-25320" yWindow="360" windowWidth="25440" windowHeight="15270" xr2:uid="{867F3169-A9A3-4AE6-89E2-304587BC45FE}"/>
   </bookViews>
   <sheets>
     <sheet name="storm2_results" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>max_amp</t>
   </si>
@@ -174,8 +174,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -660,7 +661,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -669,8 +670,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5448,14 +5455,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121C4130-64D5-42FE-8592-ED0ECA68F7E8}">
   <dimension ref="A1:CS129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA39" sqref="AA39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z41" sqref="Z41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5736,18 +5744,10 @@
       <c r="CO1" s="1">
         <v>44777.000694444447</v>
       </c>
-      <c r="CP1" s="1">
-        <v>44400.959027777775</v>
-      </c>
-      <c r="CQ1" s="1">
-        <v>44400.969444444447</v>
-      </c>
-      <c r="CR1" s="1">
-        <v>44400.979861111111</v>
-      </c>
-      <c r="CS1" s="1">
-        <v>44400.990277777775</v>
-      </c>
+      <c r="CP1" s="1"/>
+      <c r="CQ1" s="1"/>
+      <c r="CR1" s="1"/>
+      <c r="CS1" s="1"/>
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6028,18 +6028,6 @@
       </c>
       <c r="CO2">
         <v>6.3385999173041297E-3</v>
-      </c>
-      <c r="CP2">
-        <v>3.6342641577993003E-2</v>
-      </c>
-      <c r="CQ2">
-        <v>3.4873229057135302E-2</v>
-      </c>
-      <c r="CR2">
-        <v>3.3406134664429599E-2</v>
-      </c>
-      <c r="CS2">
-        <v>3.2223898770697097E-2</v>
       </c>
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.25">
@@ -6322,18 +6310,6 @@
       <c r="CO3">
         <v>4.4831709177640504E-3</v>
       </c>
-      <c r="CP3">
-        <v>3.4811107055907398E-2</v>
-      </c>
-      <c r="CQ3">
-        <v>3.3295727776517597E-2</v>
-      </c>
-      <c r="CR3">
-        <v>3.2443750861737598E-2</v>
-      </c>
-      <c r="CS3">
-        <v>3.12858073086653E-2</v>
-      </c>
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -6615,18 +6591,6 @@
       <c r="CO4">
         <v>4.33979892746463E-3</v>
       </c>
-      <c r="CP4">
-        <v>3.48162025725475E-2</v>
-      </c>
-      <c r="CQ4">
-        <v>3.32920365830328E-2</v>
-      </c>
-      <c r="CR4">
-        <v>3.2431141831294502E-2</v>
-      </c>
-      <c r="CS4">
-        <v>3.1324109053877197E-2</v>
-      </c>
     </row>
     <row r="5" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -6908,18 +6872,6 @@
       <c r="CO5">
         <v>0</v>
       </c>
-      <c r="CP5">
-        <v>0</v>
-      </c>
-      <c r="CQ5">
-        <v>0</v>
-      </c>
-      <c r="CR5">
-        <v>0</v>
-      </c>
-      <c r="CS5">
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -7201,18 +7153,6 @@
       <c r="CO6">
         <v>0</v>
       </c>
-      <c r="CP6">
-        <v>0</v>
-      </c>
-      <c r="CQ6">
-        <v>0</v>
-      </c>
-      <c r="CR6">
-        <v>0</v>
-      </c>
-      <c r="CS6">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -7494,18 +7434,6 @@
       <c r="CO7">
         <v>2</v>
       </c>
-      <c r="CP7">
-        <v>0</v>
-      </c>
-      <c r="CQ7">
-        <v>0</v>
-      </c>
-      <c r="CR7">
-        <v>0</v>
-      </c>
-      <c r="CS7">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -7787,18 +7715,6 @@
       <c r="CO8">
         <v>130</v>
       </c>
-      <c r="CP8">
-        <v>16577</v>
-      </c>
-      <c r="CQ8">
-        <v>16107</v>
-      </c>
-      <c r="CR8">
-        <v>15955</v>
-      </c>
-      <c r="CS8">
-        <v>15874</v>
-      </c>
     </row>
     <row r="9" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -8080,18 +7996,6 @@
       <c r="CO9">
         <v>3563</v>
       </c>
-      <c r="CP9">
-        <v>6401</v>
-      </c>
-      <c r="CQ9">
-        <v>6351</v>
-      </c>
-      <c r="CR9">
-        <v>6413</v>
-      </c>
-      <c r="CS9">
-        <v>6715</v>
-      </c>
     </row>
     <row r="10" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -8373,18 +8277,6 @@
       <c r="CO10">
         <v>12637</v>
       </c>
-      <c r="CP10">
-        <v>1622</v>
-      </c>
-      <c r="CQ10">
-        <v>1654</v>
-      </c>
-      <c r="CR10">
-        <v>1673</v>
-      </c>
-      <c r="CS10">
-        <v>1690</v>
-      </c>
     </row>
     <row r="11" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -8666,18 +8558,6 @@
       <c r="CO11">
         <v>0</v>
       </c>
-      <c r="CP11">
-        <v>0</v>
-      </c>
-      <c r="CQ11">
-        <v>0</v>
-      </c>
-      <c r="CR11">
-        <v>0</v>
-      </c>
-      <c r="CS11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -8959,18 +8839,6 @@
       <c r="CO12">
         <v>0</v>
       </c>
-      <c r="CP12">
-        <v>0</v>
-      </c>
-      <c r="CQ12">
-        <v>0</v>
-      </c>
-      <c r="CR12">
-        <v>0</v>
-      </c>
-      <c r="CS12">
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -9252,18 +9120,6 @@
       <c r="CO13">
         <v>0</v>
       </c>
-      <c r="CP13">
-        <v>0</v>
-      </c>
-      <c r="CQ13">
-        <v>0</v>
-      </c>
-      <c r="CR13">
-        <v>0</v>
-      </c>
-      <c r="CS13">
-        <v>0</v>
-      </c>
     </row>
     <row r="14" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -9545,18 +9401,6 @@
       <c r="CO14">
         <v>0</v>
       </c>
-      <c r="CP14">
-        <v>0</v>
-      </c>
-      <c r="CQ14">
-        <v>0</v>
-      </c>
-      <c r="CR14">
-        <v>0</v>
-      </c>
-      <c r="CS14">
-        <v>0</v>
-      </c>
     </row>
     <row r="15" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -9838,18 +9682,6 @@
       <c r="CO15">
         <v>0</v>
       </c>
-      <c r="CP15">
-        <v>0</v>
-      </c>
-      <c r="CQ15">
-        <v>0</v>
-      </c>
-      <c r="CR15">
-        <v>0</v>
-      </c>
-      <c r="CS15">
-        <v>0</v>
-      </c>
     </row>
     <row r="16" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -10131,18 +9963,6 @@
       <c r="CO16">
         <v>0</v>
       </c>
-      <c r="CP16">
-        <v>0</v>
-      </c>
-      <c r="CQ16">
-        <v>0</v>
-      </c>
-      <c r="CR16">
-        <v>0</v>
-      </c>
-      <c r="CS16">
-        <v>0</v>
-      </c>
     </row>
     <row r="17" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -10424,18 +10244,6 @@
       <c r="CO17">
         <v>8.3854042377042901E-2</v>
       </c>
-      <c r="CP17">
-        <v>0</v>
-      </c>
-      <c r="CQ17">
-        <v>0</v>
-      </c>
-      <c r="CR17">
-        <v>0</v>
-      </c>
-      <c r="CS17">
-        <v>0</v>
-      </c>
     </row>
     <row r="18" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -10717,18 +10525,6 @@
       <c r="CO18">
         <v>7.9411307859004798E-2</v>
       </c>
-      <c r="CP18">
-        <v>0</v>
-      </c>
-      <c r="CQ18">
-        <v>0</v>
-      </c>
-      <c r="CR18">
-        <v>0</v>
-      </c>
-      <c r="CS18">
-        <v>0</v>
-      </c>
     </row>
     <row r="19" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -11010,18 +10806,6 @@
       <c r="CO19">
         <v>7.9411307859004798E-2</v>
       </c>
-      <c r="CP19">
-        <v>0</v>
-      </c>
-      <c r="CQ19">
-        <v>0</v>
-      </c>
-      <c r="CR19">
-        <v>0</v>
-      </c>
-      <c r="CS19">
-        <v>0</v>
-      </c>
     </row>
     <row r="20" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -11303,18 +11087,6 @@
       <c r="CO20">
         <v>0.40567039470746402</v>
       </c>
-      <c r="CP20">
-        <v>2.3259290609915499</v>
-      </c>
-      <c r="CQ20">
-        <v>2.23188665965665</v>
-      </c>
-      <c r="CR20">
-        <v>2.1379926185234899</v>
-      </c>
-      <c r="CS20">
-        <v>2.0623295213246098</v>
-      </c>
     </row>
     <row r="21" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -11596,18 +11368,6 @@
       <c r="CO21">
         <v>0.29748097307454302</v>
       </c>
-      <c r="CP21">
-        <v>2.2279108515780699</v>
-      </c>
-      <c r="CQ21">
-        <v>2.13092657769712</v>
-      </c>
-      <c r="CR21">
-        <v>2.0764000551512001</v>
-      </c>
-      <c r="CS21">
-        <v>2.0022916677545801</v>
-      </c>
     </row>
     <row r="22" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -11889,18 +11649,6 @@
       <c r="CO22">
         <v>0.285269908796973</v>
       </c>
-      <c r="CP22">
-        <v>2.22823696464304</v>
-      </c>
-      <c r="CQ22">
-        <v>2.1306903413141001</v>
-      </c>
-      <c r="CR22">
-        <v>2.0755930772028499</v>
-      </c>
-      <c r="CS22">
-        <v>2.0047429794481402</v>
-      </c>
     </row>
     <row r="23" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -12182,18 +11930,6 @@
       <c r="CO23">
         <v>1.6226815788298501</v>
       </c>
-      <c r="CP23">
-        <v>9.3037162439662104</v>
-      </c>
-      <c r="CQ23">
-        <v>8.9275466386266302</v>
-      </c>
-      <c r="CR23">
-        <v>8.5519704740939897</v>
-      </c>
-      <c r="CS23">
-        <v>8.2493180852984693</v>
-      </c>
     </row>
     <row r="24" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -12475,18 +12211,6 @@
       <c r="CO24">
         <v>1.14769175494759</v>
       </c>
-      <c r="CP24">
-        <v>8.9116434063122991</v>
-      </c>
-      <c r="CQ24">
-        <v>8.5237063107885103</v>
-      </c>
-      <c r="CR24">
-        <v>8.3056002206048198</v>
-      </c>
-      <c r="CS24">
-        <v>8.0091666710183205</v>
-      </c>
     </row>
     <row r="25" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -12768,18 +12492,6 @@
       <c r="CO25">
         <v>1.11098852543094</v>
       </c>
-      <c r="CP25">
-        <v>8.9129478585721706</v>
-      </c>
-      <c r="CQ25">
-        <v>8.5227613652564091</v>
-      </c>
-      <c r="CR25">
-        <v>8.3023723088114103</v>
-      </c>
-      <c r="CS25">
-        <v>8.0189719177925607</v>
-      </c>
     </row>
     <row r="26" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -13061,18 +12773,6 @@
       <c r="CO26">
         <v>6.4907263153194297</v>
       </c>
-      <c r="CP26">
-        <v>37.214864975864799</v>
-      </c>
-      <c r="CQ26">
-        <v>35.7101865545065</v>
-      </c>
-      <c r="CR26">
-        <v>34.207881896375902</v>
-      </c>
-      <c r="CS26">
-        <v>32.997272341193899</v>
-      </c>
     </row>
     <row r="27" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -13354,18 +13054,6 @@
       <c r="CO27">
         <v>4.5907670197903903</v>
       </c>
-      <c r="CP27">
-        <v>35.646573625249196</v>
-      </c>
-      <c r="CQ27">
-        <v>34.094825243153998</v>
-      </c>
-      <c r="CR27">
-        <v>33.222400882419301</v>
-      </c>
-      <c r="CS27">
-        <v>32.036666684073197</v>
-      </c>
     </row>
     <row r="28" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -13647,18 +13335,6 @@
       <c r="CO28">
         <v>4.44395410172379</v>
       </c>
-      <c r="CP28">
-        <v>35.651791434288697</v>
-      </c>
-      <c r="CQ28">
-        <v>34.091045461025601</v>
-      </c>
-      <c r="CR28">
-        <v>33.209489235245599</v>
-      </c>
-      <c r="CS28">
-        <v>32.0758876711702</v>
-      </c>
     </row>
     <row r="29" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -13940,18 +13616,6 @@
       <c r="CO29">
         <v>2.2059633774999998</v>
       </c>
-      <c r="CP29">
-        <v>33.70122155</v>
-      </c>
-      <c r="CQ29">
-        <v>32.481755229999997</v>
-      </c>
-      <c r="CR29">
-        <v>31.422086315000001</v>
-      </c>
-      <c r="CS29">
-        <v>30.459591920000001</v>
-      </c>
     </row>
     <row r="30" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -14233,18 +13897,6 @@
       <c r="CO30">
         <v>11.596826141446799</v>
       </c>
-      <c r="CP30">
-        <v>364.64324160199999</v>
-      </c>
-      <c r="CQ30">
-        <v>351.42422669319899</v>
-      </c>
-      <c r="CR30">
-        <v>339.93741565459999</v>
-      </c>
-      <c r="CS30">
-        <v>329.5039764128</v>
-      </c>
     </row>
     <row r="31" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -14526,18 +14178,10 @@
       <c r="CO31" s="1">
         <v>44777.000694444447</v>
       </c>
-      <c r="CP31" s="1">
-        <v>44400.959027777775</v>
-      </c>
-      <c r="CQ31" s="1">
-        <v>44400.969444444447</v>
-      </c>
-      <c r="CR31" s="1">
-        <v>44400.979861111111</v>
-      </c>
-      <c r="CS31" s="1">
-        <v>44400.990277777775</v>
-      </c>
+      <c r="CP31" s="1"/>
+      <c r="CQ31" s="1"/>
+      <c r="CR31" s="1"/>
+      <c r="CS31" s="1"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C33" s="4" t="s">
@@ -14561,13 +14205,13 @@
         <f>A2</f>
         <v>max_amp</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="9">
         <f>MAX(B2:CS2)</f>
-        <v>3.6342641577993003E-2</v>
-      </c>
-      <c r="C34" s="7">
+        <v>2.7100659833378001E-2</v>
+      </c>
+      <c r="C34" s="6">
         <f>_xlfn.XLOOKUP(MAX(B2:CS2), B2:CS2, $B$1:$CS$1)</f>
-        <v>44400.959027777775</v>
+        <v>44776.625694444447</v>
       </c>
       <c r="E34" s="1">
         <v>44776.000694444447</v>
@@ -14587,13 +14231,13 @@
         <f t="shared" ref="A35:A60" si="0">A3</f>
         <v>mean_amp</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="9">
         <f t="shared" ref="B35:B60" si="1">MAX(B3:CS3)</f>
-        <v>3.4811107055907398E-2</v>
-      </c>
-      <c r="C35" s="7">
-        <f t="shared" ref="C35:C60" si="2">_xlfn.XLOOKUP(MAX(B3:CS3), B3:CS3, $B$1:$CS$1)</f>
-        <v>44400.959027777775</v>
+        <v>1.73415591077304E-2</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" ref="C35:C59" si="2">_xlfn.XLOOKUP(MAX(B3:CS3), B3:CS3, $B$1:$CS$1)</f>
+        <v>44776.625694444447</v>
       </c>
       <c r="E35" s="1">
         <v>44776.011111111111</v>
@@ -14611,7 +14255,7 @@
         <v>0</v>
       </c>
       <c r="U35">
-        <v>3.6342641577993003E-2</v>
+        <v>2.7100659833378001E-2</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
@@ -14619,13 +14263,13 @@
         <f t="shared" si="0"/>
         <v>median_amp</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="9">
         <f t="shared" si="1"/>
-        <v>3.48162025725475E-2</v>
-      </c>
-      <c r="C36" s="7">
+        <v>1.75334302078048E-2</v>
+      </c>
+      <c r="C36" s="6">
         <f t="shared" si="2"/>
-        <v>44400.959027777775</v>
+        <v>44776.625694444447</v>
       </c>
       <c r="E36" s="1">
         <v>44776.021527777775</v>
@@ -14643,7 +14287,7 @@
         <v>1</v>
       </c>
       <c r="U36">
-        <v>3.4811107055907398E-2</v>
+        <v>1.73415591077304E-2</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
@@ -14651,7 +14295,7 @@
         <f t="shared" si="0"/>
         <v>impulses_ch6</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -14675,7 +14319,7 @@
         <v>2</v>
       </c>
       <c r="U37">
-        <v>3.48162025725475E-2</v>
+        <v>1.75334302078048E-2</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
@@ -14683,7 +14327,7 @@
         <f t="shared" si="0"/>
         <v>impulses_ch5</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
@@ -14715,7 +14359,7 @@
         <f t="shared" si="0"/>
         <v>impulses_ch4</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39">
         <f t="shared" si="1"/>
         <v>199</v>
       </c>
@@ -14747,13 +14391,13 @@
         <f t="shared" si="0"/>
         <v>impulses_ch3</v>
       </c>
-      <c r="B40" s="6">
-        <f t="shared" si="1"/>
-        <v>16577</v>
-      </c>
-      <c r="C40" s="7">
+      <c r="B40" s="5">
+        <f>MAX(B8:CO8)</f>
+        <v>2627</v>
+      </c>
+      <c r="C40" s="6">
         <f t="shared" si="2"/>
-        <v>44400.959027777775</v>
+        <v>44776.625694444447</v>
       </c>
       <c r="E40" s="1">
         <v>44776.063194444447</v>
@@ -14779,11 +14423,11 @@
         <f t="shared" si="0"/>
         <v>impulses_ch2</v>
       </c>
-      <c r="B41" s="6">
-        <f t="shared" si="1"/>
+      <c r="B41" s="5">
+        <f t="shared" ref="B41:B42" si="3">MAX(B9:CO9)</f>
         <v>11852</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="6">
         <f t="shared" si="2"/>
         <v>44776.636111111111</v>
       </c>
@@ -14803,7 +14447,7 @@
         <v>6</v>
       </c>
       <c r="U41">
-        <v>16577</v>
+        <v>2627</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
@@ -14811,11 +14455,11 @@
         <f t="shared" si="0"/>
         <v>impulses_ch1</v>
       </c>
-      <c r="B42" s="6">
-        <f t="shared" si="1"/>
+      <c r="B42" s="5">
+        <f t="shared" si="3"/>
         <v>15119</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="6">
         <f t="shared" si="2"/>
         <v>44776.802777777775</v>
       </c>
@@ -14843,7 +14487,7 @@
         <f t="shared" si="0"/>
         <v>max_env_ch6</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -14875,7 +14519,7 @@
         <f t="shared" si="0"/>
         <v>mean_env_ch6</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -14901,7 +14545,7 @@
         <f t="shared" si="0"/>
         <v>median_env_ch6</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -14930,7 +14574,7 @@
         <f t="shared" si="0"/>
         <v>max_env_ch5</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46">
         <f t="shared" si="1"/>
         <v>0.108402639333512</v>
       </c>
@@ -14974,7 +14618,7 @@
         <f t="shared" si="0"/>
         <v>mean_env_ch5</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47">
         <f t="shared" si="1"/>
         <v>8.5195492688122099E-2</v>
       </c>
@@ -15024,7 +14668,7 @@
         <f t="shared" si="0"/>
         <v>median_env_ch5</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48">
         <f t="shared" si="1"/>
         <v>8.1549751061042799E-2</v>
       </c>
@@ -15074,7 +14718,7 @@
         <f t="shared" si="0"/>
         <v>max_env_ch4</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49">
         <f t="shared" si="1"/>
         <v>0.43361055733404802</v>
       </c>
@@ -15124,7 +14768,7 @@
         <f t="shared" si="0"/>
         <v>mean_env_ch4</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50">
         <f t="shared" si="1"/>
         <v>0.283546008743847</v>
       </c>
@@ -15149,15 +14793,15 @@
       </c>
       <c r="U50" s="2">
         <f>B52</f>
-        <v>2.3259290609915499</v>
+        <v>1.7344422293361901</v>
       </c>
       <c r="V50" s="2">
         <f>B53</f>
-        <v>2.2279108515780699</v>
+        <v>1.1098597828947401</v>
       </c>
       <c r="W50" s="2">
         <f>B54</f>
-        <v>2.22823696464304</v>
+        <v>1.1221395332995101</v>
       </c>
       <c r="Y50">
         <v>2.3259290609915499</v>
@@ -15174,7 +14818,7 @@
         <f t="shared" si="0"/>
         <v>median_env_ch4</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51">
         <f t="shared" si="1"/>
         <v>0.28905210154241401</v>
       </c>
@@ -15199,15 +14843,15 @@
       </c>
       <c r="U51" s="2">
         <f>B55</f>
-        <v>9.3037162439662104</v>
+        <v>6.9377689173447701</v>
       </c>
       <c r="V51" s="2">
         <f>B56</f>
-        <v>8.9116434063122991</v>
+        <v>4.4394391315789896</v>
       </c>
       <c r="W51" s="2">
         <f>B57</f>
-        <v>8.9129478585721706</v>
+        <v>4.4885581331980502</v>
       </c>
       <c r="Y51">
         <v>9.3037162439662104</v>
@@ -15224,13 +14868,13 @@
         <f t="shared" si="0"/>
         <v>max_env_ch3</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="5">
         <f t="shared" si="1"/>
-        <v>2.3259290609915499</v>
-      </c>
-      <c r="C52" s="7">
+        <v>1.7344422293361901</v>
+      </c>
+      <c r="C52" s="6">
         <f t="shared" si="2"/>
-        <v>44400.959027777775</v>
+        <v>44776.625694444447</v>
       </c>
       <c r="E52" s="1">
         <v>44776.188194444447</v>
@@ -15249,15 +14893,15 @@
       </c>
       <c r="U52" s="2">
         <f>B58</f>
-        <v>37.214864975864799</v>
+        <v>27.751075669378999</v>
       </c>
       <c r="V52" s="2">
         <f>B59</f>
-        <v>35.646573625249196</v>
+        <v>17.757756526315902</v>
       </c>
       <c r="W52" s="2">
         <f>B60</f>
-        <v>35.651791434288697</v>
+        <v>17.954232532792201</v>
       </c>
       <c r="Y52">
         <v>37.214864975864799</v>
@@ -15274,13 +14918,13 @@
         <f t="shared" si="0"/>
         <v>mean_env_ch3</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="5">
         <f t="shared" si="1"/>
-        <v>2.2279108515780699</v>
-      </c>
-      <c r="C53" s="7">
+        <v>1.1098597828947401</v>
+      </c>
+      <c r="C53" s="6">
         <f t="shared" si="2"/>
-        <v>44400.959027777775</v>
+        <v>44776.625694444447</v>
       </c>
       <c r="E53" s="1">
         <v>44776.198611111111</v>
@@ -15300,13 +14944,13 @@
         <f t="shared" si="0"/>
         <v>median_env_ch3</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="5">
         <f t="shared" si="1"/>
-        <v>2.22823696464304</v>
-      </c>
-      <c r="C54" s="7">
+        <v>1.1221395332995101</v>
+      </c>
+      <c r="C54" s="6">
         <f t="shared" si="2"/>
-        <v>44400.959027777775</v>
+        <v>44776.625694444447</v>
       </c>
       <c r="E54" s="1">
         <v>44776.209027777775</v>
@@ -15326,13 +14970,13 @@
         <f t="shared" si="0"/>
         <v>max_env_ch2</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="5">
         <f t="shared" si="1"/>
-        <v>9.3037162439662104</v>
-      </c>
-      <c r="C55" s="7">
+        <v>6.9377689173447701</v>
+      </c>
+      <c r="C55" s="6">
         <f t="shared" si="2"/>
-        <v>44400.959027777775</v>
+        <v>44776.625694444447</v>
       </c>
       <c r="E55" s="1">
         <v>44776.219444444447</v>
@@ -15352,13 +14996,13 @@
         <f t="shared" si="0"/>
         <v>mean_env_ch2</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="5">
         <f t="shared" si="1"/>
-        <v>8.9116434063122991</v>
-      </c>
-      <c r="C56" s="7">
+        <v>4.4394391315789896</v>
+      </c>
+      <c r="C56" s="6">
         <f t="shared" si="2"/>
-        <v>44400.959027777775</v>
+        <v>44776.625694444447</v>
       </c>
       <c r="E56" s="1">
         <v>44776.229861111111</v>
@@ -15378,13 +15022,13 @@
         <f t="shared" si="0"/>
         <v>median_env_ch2</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="5">
         <f t="shared" si="1"/>
-        <v>8.9129478585721706</v>
-      </c>
-      <c r="C57" s="7">
+        <v>4.4885581331980502</v>
+      </c>
+      <c r="C57" s="6">
         <f t="shared" si="2"/>
-        <v>44400.959027777775</v>
+        <v>44776.625694444447</v>
       </c>
       <c r="E57" s="1">
         <v>44776.240277777775</v>
@@ -15404,13 +15048,13 @@
         <f t="shared" si="0"/>
         <v>max_env_ch1</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="5">
         <f t="shared" si="1"/>
-        <v>37.214864975864799</v>
-      </c>
-      <c r="C58" s="7">
+        <v>27.751075669378999</v>
+      </c>
+      <c r="C58" s="6">
         <f t="shared" si="2"/>
-        <v>44400.959027777775</v>
+        <v>44776.625694444447</v>
       </c>
       <c r="E58" s="1">
         <v>44776.250694444447</v>
@@ -15430,13 +15074,13 @@
         <f t="shared" si="0"/>
         <v>mean_env_ch1</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="5">
         <f t="shared" si="1"/>
-        <v>35.646573625249196</v>
-      </c>
-      <c r="C59" s="7">
+        <v>17.757756526315902</v>
+      </c>
+      <c r="C59" s="6">
         <f t="shared" si="2"/>
-        <v>44400.959027777775</v>
+        <v>44776.625694444447</v>
       </c>
       <c r="E59" s="1">
         <v>44776.261111111111</v>
@@ -15456,13 +15100,13 @@
         <f t="shared" si="0"/>
         <v>median_env_ch1</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="5">
         <f t="shared" si="1"/>
-        <v>35.651791434288697</v>
-      </c>
-      <c r="C60" s="7">
-        <f t="shared" si="2"/>
-        <v>44400.959027777775</v>
+        <v>17.954232532792201</v>
+      </c>
+      <c r="C60" s="6">
+        <f>_xlfn.XLOOKUP(MAX(B28:CS28), B28:CS28, $B$1:$CS$1)</f>
+        <v>44776.625694444447</v>
       </c>
       <c r="E60" s="1">
         <v>44776.271527777775</v>
@@ -15478,6 +15122,17 @@
       </c>
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" s="7">
+        <f>MAX(B29:CS29)</f>
+        <v>22.620213794999898</v>
+      </c>
+      <c r="C61" s="6">
+        <f t="shared" ref="C61:C62" si="4">_xlfn.XLOOKUP(MAX(B29:CS29), B29:CS29, $B$1:$CS$1)</f>
+        <v>44776.636111111111</v>
+      </c>
       <c r="E61" s="1">
         <v>44776.281944444447</v>
       </c>
@@ -15492,6 +15147,17 @@
       </c>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" s="7">
+        <f>MAX(B30:CS30)</f>
+        <v>22.364671984258202</v>
+      </c>
+      <c r="C62" s="6">
+        <f t="shared" si="4"/>
+        <v>44776.636111111111</v>
+      </c>
       <c r="E62" s="1">
         <v>44776.292361111111</v>
       </c>
@@ -15506,6 +15172,8 @@
       </c>
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B63" s="8"/>
+      <c r="C63" s="3"/>
       <c r="E63" s="1">
         <v>44776.302777777775</v>
       </c>

</xml_diff>